<commit_message>
opportunite daffaire concurrence et cout
</commit_message>
<xml_diff>
--- a/CR/FarView-Analyse des coûts.xlsx
+++ b/CR/FarView-Analyse des coûts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="28515" windowHeight="12075"/>
+    <workbookView xWindow="120" yWindow="72" windowWidth="23256" windowHeight="12072"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>1 an</t>
   </si>
@@ -42,18 +42,12 @@
     <t>Communication</t>
   </si>
   <si>
-    <t>Salaires fondateurs (4 personnes)</t>
-  </si>
-  <si>
     <t>Impôts</t>
   </si>
   <si>
     <t>Charges annuelles (€/an)</t>
   </si>
   <si>
-    <t>Investissment annuel (€/an)</t>
-  </si>
-  <si>
     <t>Hébergement site internet</t>
   </si>
   <si>
@@ -66,9 +60,6 @@
     <t>Location locaux 60m²</t>
   </si>
   <si>
-    <t>Charges locaux (électricité, eau)</t>
-  </si>
-  <si>
     <t>Commercial</t>
   </si>
   <si>
@@ -118,6 +109,24 @@
   </si>
   <si>
     <t>Fourniture bureau (dont imprimante)</t>
+  </si>
+  <si>
+    <t>Investissement annuel (€/an)</t>
+  </si>
+  <si>
+    <t>Charges locaux (électricité, eau, internet)</t>
+  </si>
+  <si>
+    <t>Honoraire avocat</t>
+  </si>
+  <si>
+    <t>Salaires fondateurs (4 personnes)*</t>
+  </si>
+  <si>
+    <t>Développeur supplémentaire</t>
+  </si>
+  <si>
+    <t>*Les 4 fondateurs sont principalement développeurs, et peuvent occasionnelement gérer d'autres domaines. (conception des tutoriels vidéos, rédaction d'articles, rédaction du site…)</t>
   </si>
 </sst>
 </file>
@@ -317,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -346,24 +355,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -378,6 +369,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,83 +752,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:J37"/>
+  <dimension ref="A3:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" style="2" customWidth="1"/>
-    <col min="2" max="6" width="11.42578125" style="1"/>
-    <col min="7" max="7" width="30.7109375" style="2" customWidth="1"/>
-    <col min="8" max="9" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="36.6640625" style="2" customWidth="1"/>
+    <col min="2" max="6" width="11.44140625" style="1"/>
+    <col min="7" max="7" width="30.6640625" style="2" customWidth="1"/>
+    <col min="8" max="9" width="11.44140625" style="1"/>
     <col min="10" max="10" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="1"/>
+    <col min="11" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F3" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="15"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F4" s="16"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="18"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F3" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="21"/>
+      <c r="H3" s="22"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F4" s="23"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="26" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="12" t="s">
         <v>23</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
-        <v>26</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="G9" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H9" s="8">
         <v>3500</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1">
         <v>100</v>
@@ -813,9 +837,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
@@ -834,15 +858,15 @@
         <v>500</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1">
         <v>200</v>
@@ -854,17 +878,26 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>16</v>
+        <v>32</v>
+      </c>
+      <c r="B13" s="1">
+        <v>350</v>
+      </c>
+      <c r="C13" s="1">
+        <v>500</v>
+      </c>
+      <c r="D13" s="1">
+        <v>590</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1">
         <f>5*12</f>
@@ -878,7 +911,7 @@
         <v>120</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H14" s="1">
         <v>100</v>
@@ -890,9 +923,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B15" s="1">
         <f>1500+4*250</f>
@@ -908,17 +941,20 @@
       </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="1">
+        <v>500</v>
+      </c>
       <c r="G16" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>2</v>
-      </c>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="G17" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H17" s="1">
         <v>0</v>
@@ -927,24 +963,15 @@
         <v>4000</v>
       </c>
       <c r="J17" s="1">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="1">
-        <v>50</v>
-      </c>
-      <c r="C18" s="1">
-        <v>100</v>
-      </c>
-      <c r="D18" s="1">
-        <v>150</v>
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
+        <v>2</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H18" s="1">
         <v>0</v>
@@ -956,198 +983,248 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="1">
+        <v>50</v>
+      </c>
+      <c r="C19" s="1">
+        <v>100</v>
+      </c>
+      <c r="D19" s="1">
+        <v>150</v>
+      </c>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B20" s="1">
         <v>0</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C20" s="1">
         <f>20*12</f>
         <v>240</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D20" s="1">
         <f>20*12</f>
         <v>240</v>
       </c>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+    </row>
+    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B22" s="1">
         <f>3*2000</f>
         <v>6000</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C22" s="1">
         <f>3*2000</f>
         <v>6000</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D22" s="1">
         <f>3*2000</f>
         <v>6000</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+    <row r="23" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="11"/>
+    </row>
+    <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="1">
+    <row r="25" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="1">
         <v>40</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C25" s="1">
         <f>4*60000</f>
         <v>240000</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D25" s="1">
         <f>4*70000</f>
         <v>280000</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="1">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="1">
         <v>0</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C26" s="1">
         <v>40000</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D26" s="1">
         <v>40000</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
+    <row r="30" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B30" s="1">
         <v>100</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C30" s="1">
         <v>200</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D30" s="1">
         <v>400</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="1">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="1">
         <v>100</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C31" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" s="1">
+        <v>250</v>
+      </c>
+      <c r="C35" s="1">
         <v>500</v>
       </c>
-      <c r="D29" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="1">
-        <v>250</v>
-      </c>
-      <c r="C33" s="1">
-        <v>500</v>
-      </c>
-      <c r="D33" s="1">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="19"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="21"/>
-    </row>
-    <row r="36" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" s="22">
-        <f t="shared" ref="B36:D36" si="0">SUM(B9:B35)</f>
-        <v>9400</v>
-      </c>
-      <c r="C36" s="23">
-        <f t="shared" si="0"/>
-        <v>296850</v>
-      </c>
-      <c r="D36" s="23">
-        <f t="shared" si="0"/>
-        <v>338160</v>
-      </c>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H36" s="23">
-        <f>SUM(H9:H35)</f>
+      <c r="D35" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="13"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="15"/>
+    </row>
+    <row r="38" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" s="16">
+        <f>SUM(B9:B37)</f>
+        <v>10250</v>
+      </c>
+      <c r="C38" s="17">
+        <f>SUM(C9:C37)</f>
+        <v>298850</v>
+      </c>
+      <c r="D38" s="17">
+        <f>SUM(D9:D37)</f>
+        <v>398950</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H38" s="17">
+        <f>SUM(H9:H37)</f>
         <v>4100</v>
       </c>
-      <c r="I36" s="23">
-        <f>SUM(I9:I35)</f>
+      <c r="I38" s="17">
+        <f>SUM(I9:I37)</f>
         <v>4500</v>
       </c>
-      <c r="J36" s="22">
-        <f>SUM(J9:J35)</f>
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
+      <c r="J38" s="16">
+        <f>SUM(J9:J37)</f>
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" s="28"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="28"/>
+      <c r="H43" s="28"/>
+      <c r="I43" s="28"/>
+      <c r="J43" s="29"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="30"/>
+      <c r="B44" s="31"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="F3:H4"/>
+    <mergeCell ref="A43:J43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1161,7 +1238,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1173,7 +1250,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ajout dee  ce qu'on doit mettre.docx
</commit_message>
<xml_diff>
--- a/CR/FarView-Analyse des coûts.xlsx
+++ b/CR/FarView-Analyse des coûts.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>1 an</t>
   </si>
@@ -51,15 +51,9 @@
     <t>Charges annuelles (€/an)</t>
   </si>
   <si>
-    <t>Investissment annuel (€/an)</t>
-  </si>
-  <si>
     <t>Hébergement site internet</t>
   </si>
   <si>
-    <t>Téléphone</t>
-  </si>
-  <si>
     <t>Location locaux "boite au lettre"</t>
   </si>
   <si>
@@ -118,6 +112,18 @@
   </si>
   <si>
     <t>Fourniture bureau (dont imprimante)</t>
+  </si>
+  <si>
+    <t>Téléphone, internet</t>
+  </si>
+  <si>
+    <t>Avocat</t>
+  </si>
+  <si>
+    <t>Investissement annuel (€/an)</t>
+  </si>
+  <si>
+    <t>Mobilier</t>
   </si>
 </sst>
 </file>
@@ -347,24 +353,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -377,6 +365,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -728,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:J37"/>
+  <dimension ref="A3:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,16 +751,16 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F3" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="15"/>
+      <c r="F3" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="21"/>
+      <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F4" s="16"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="18"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
@@ -764,50 +770,50 @@
         <v>0</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>0</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="G9" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H9" s="8">
         <v>3500</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
@@ -815,7 +821,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
@@ -834,15 +840,15 @@
         <v>500</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1">
         <v>200</v>
@@ -856,7 +862,16 @@
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="B13" s="1">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1">
+        <v>400</v>
+      </c>
+      <c r="D13" s="1">
+        <v>400</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>7</v>
@@ -864,21 +879,20 @@
     </row>
     <row r="14" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B14" s="1">
-        <f>5*12</f>
-        <v>60</v>
+        <v>300</v>
       </c>
       <c r="C14" s="1">
-        <v>60</v>
+        <v>300</v>
       </c>
       <c r="D14" s="1">
         <f>2*B14</f>
-        <v>120</v>
+        <v>600</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H14" s="1">
         <v>100</v>
@@ -892,7 +906,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15" s="1">
         <f>1500+4*250</f>
@@ -909,16 +923,25 @@
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="1">
+        <v>500</v>
+      </c>
+      <c r="C16" s="1">
+        <v>500</v>
+      </c>
+      <c r="D16" s="1">
+        <v>500</v>
+      </c>
       <c r="G16" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>2</v>
-      </c>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="G17" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H17" s="1">
         <v>0</v>
@@ -930,21 +953,12 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="1">
-        <v>50</v>
-      </c>
-      <c r="C18" s="1">
-        <v>100</v>
-      </c>
-      <c r="D18" s="1">
-        <v>150</v>
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>2</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H18" s="1">
         <v>0</v>
@@ -956,194 +970,215 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="1">
+        <v>60</v>
+      </c>
+      <c r="C19" s="1">
+        <v>120</v>
+      </c>
+      <c r="D19" s="1">
+        <v>150</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1">
+        <v>4000</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B20" s="1">
         <v>0</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C20" s="1">
         <f>20*12</f>
         <v>240</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D20" s="1">
         <f>20*12</f>
         <v>240</v>
       </c>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+    </row>
+    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B22" s="1">
         <f>3*2000</f>
         <v>6000</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C22" s="1">
         <f>3*2000</f>
         <v>6000</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D22" s="1">
         <f>3*2000</f>
         <v>6000</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+    <row r="23" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+    <row r="25" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B25" s="1">
         <v>40</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C25" s="1">
         <f>4*60000</f>
         <v>240000</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D25" s="1">
         <f>4*70000</f>
         <v>280000</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="1">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="1">
         <v>0</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C26" s="1">
         <v>40000</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D26" s="1">
         <v>40000</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
+    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
+    <row r="29" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
         <v>6</v>
-      </c>
-      <c r="B28" s="1">
-        <v>100</v>
-      </c>
-      <c r="C28" s="1">
-        <v>200</v>
-      </c>
-      <c r="D28" s="1">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="B29" s="1">
         <v>100</v>
       </c>
       <c r="C29" s="1">
+        <v>200</v>
+      </c>
+      <c r="D29" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="1">
+        <v>2600</v>
+      </c>
+      <c r="C30" s="1">
+        <v>5000</v>
+      </c>
+      <c r="D30" s="1">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="2">
+        <v>200</v>
+      </c>
+      <c r="C32" s="2">
+        <v>300</v>
+      </c>
+      <c r="D32" s="2">
         <v>500</v>
       </c>
-      <c r="D29" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="1">
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="1">
         <v>250</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C34" s="1">
         <v>500</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D34" s="1">
         <v>500</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="19"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="21"/>
-    </row>
-    <row r="36" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" s="22">
-        <f t="shared" ref="B36:D36" si="0">SUM(B9:B35)</f>
-        <v>9400</v>
-      </c>
-      <c r="C36" s="23">
-        <f t="shared" si="0"/>
-        <v>296850</v>
-      </c>
-      <c r="D36" s="23">
-        <f t="shared" si="0"/>
-        <v>338160</v>
-      </c>
+    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="13"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
-      <c r="G36" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H36" s="23">
-        <f>SUM(H9:H35)</f>
-        <v>4100</v>
-      </c>
-      <c r="I36" s="23">
-        <f>SUM(I9:I35)</f>
-        <v>4500</v>
-      </c>
-      <c r="J36" s="22">
-        <f>SUM(J9:J35)</f>
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="15"/>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="16">
+        <f>SUM(B9:B36)</f>
+        <v>12880</v>
+      </c>
+      <c r="C37" s="17">
+        <f>SUM(C9:C36)</f>
+        <v>302810</v>
+      </c>
+      <c r="D37" s="17">
+        <f>SUM(D9:D36)</f>
+        <v>343040</v>
+      </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
+      <c r="G37" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H37" s="17">
+        <f>SUM(H9:H36)</f>
+        <v>4100</v>
+      </c>
+      <c r="I37" s="17">
+        <f>SUM(I9:I36)</f>
+        <v>8500</v>
+      </c>
+      <c r="J37" s="16">
+        <f>SUM(J9:J36)</f>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G38" s="3"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>